<commit_message>
start project - BAIMURA - done! need to collect in one universal file
</commit_message>
<xml_diff>
--- a/my_new_book.xlsx
+++ b/my_new_book.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A3:U151"/>
+  <dimension ref="A3:AA151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>241</t>
+          <t>229</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -508,17 +508,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>35.24</t>
+          <t>37.12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G4" s="1" t="n">
@@ -566,31 +566,49 @@
       <c r="U4" t="n">
         <v>13003560</v>
       </c>
+      <c r="V4" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W4" s="2" t="n">
+        <v>509000</v>
+      </c>
+      <c r="X4" t="n">
+        <v>18894080</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>509000</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>18894080</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>239</t>
+          <t>132</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>60.61</t>
+          <t>37.13</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G5" s="1" t="n">
@@ -638,31 +656,49 @@
       <c r="U5" t="n">
         <v>21758990</v>
       </c>
+      <c r="V5" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W5" s="2" t="n">
+        <v>509000</v>
+      </c>
+      <c r="X5" t="n">
+        <v>18899170</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>509000</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>18899170</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>238</t>
+          <t>230</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>91.11</t>
+          <t>37.14</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G6" s="1" t="n">
@@ -710,31 +746,49 @@
       <c r="U6" t="n">
         <v>32526270</v>
       </c>
+      <c r="V6" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <v>509000</v>
+      </c>
+      <c r="X6" t="n">
+        <v>18904260</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>509000</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>18904260</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>234</t>
+          <t>316</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>70.97</t>
+          <t>37.46</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">7 </t>
         </is>
       </c>
       <c r="G7" s="1" t="n">
@@ -782,31 +836,49 @@
       <c r="U7" t="n">
         <v>25407260</v>
       </c>
+      <c r="V7" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W7" s="2" t="n">
+        <v>509000</v>
+      </c>
+      <c r="X7" t="n">
+        <v>19067140</v>
+      </c>
+      <c r="Y7" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>509000</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>19067140</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>232</t>
+          <t>186</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>91.11</t>
+          <t>39.32</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">7 </t>
+          <t xml:space="preserve">2  </t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G8" s="1" t="n">
@@ -854,31 +926,49 @@
       <c r="U8" t="n">
         <v>30977400</v>
       </c>
+      <c r="V8" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W8" s="2" t="n">
+        <v>499000</v>
+      </c>
+      <c r="X8" t="n">
+        <v>19620680</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>499000</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>19620680</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>228</t>
+          <t>130</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>70.97</t>
+          <t>38.95</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve">7 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G9" s="1" t="n">
@@ -926,31 +1016,49 @@
       <c r="U9" t="n">
         <v>22994280</v>
       </c>
+      <c r="V9" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <v>504000</v>
+      </c>
+      <c r="X9" t="n">
+        <v>19630800</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>504000</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>19630800</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>227</t>
+          <t>133</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>60.61</t>
+          <t>39.25</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">7 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G10" s="1" t="n">
@@ -998,31 +1106,49 @@
       <c r="U10" t="n">
         <v>20728620</v>
       </c>
+      <c r="V10" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W10" s="2" t="n">
+        <v>504000</v>
+      </c>
+      <c r="X10" t="n">
+        <v>19782000</v>
+      </c>
+      <c r="Y10" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>504000</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>19782000</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>226</t>
+          <t>124</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>91.11</t>
+          <t>38.95</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve">6 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G11" s="1" t="n">
@@ -1070,31 +1196,49 @@
       <c r="U11" t="n">
         <v>32981820</v>
       </c>
+      <c r="V11" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W11" s="2" t="n">
+        <v>519000</v>
+      </c>
+      <c r="X11" t="n">
+        <v>20215050</v>
+      </c>
+      <c r="Y11" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>519000</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>20215050</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>222</t>
+          <t>301</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>70.97</t>
+          <t>39.47</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve">6 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">7 </t>
         </is>
       </c>
       <c r="G12" s="1" t="n">
@@ -1142,31 +1286,49 @@
       <c r="U12" t="n">
         <v>25265320</v>
       </c>
+      <c r="V12" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W12" s="2" t="n">
+        <v>514000</v>
+      </c>
+      <c r="X12" t="n">
+        <v>20287580</v>
+      </c>
+      <c r="Y12" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>514000</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>20287580</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>216</t>
+          <t>283</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>68.24</t>
+          <t>39.47</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve">5 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">7 </t>
         </is>
       </c>
       <c r="G13" s="1" t="n">
@@ -1214,31 +1376,49 @@
       <c r="U13" t="n">
         <v>24361680</v>
       </c>
+      <c r="V13" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W13" s="2" t="n">
+        <v>514000</v>
+      </c>
+      <c r="X13" t="n">
+        <v>20287580</v>
+      </c>
+      <c r="Y13" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>514000</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>20287580</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>214</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>89.51</t>
+          <t>39.1</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G14" s="1" t="n">
@@ -1286,31 +1466,49 @@
       <c r="U14" t="n">
         <v>32402620</v>
       </c>
+      <c r="V14" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W14" s="2" t="n">
+        <v>519000</v>
+      </c>
+      <c r="X14" t="n">
+        <v>20292900</v>
+      </c>
+      <c r="Y14" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>519000</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>20292900</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>210</t>
+          <t>46</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>68.24</t>
+          <t>40.72</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G15" s="1" t="n">
@@ -1358,31 +1556,49 @@
       <c r="U15" t="n">
         <v>23952240</v>
       </c>
+      <c r="V15" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W15" s="2" t="n">
+        <v>499000</v>
+      </c>
+      <c r="X15" t="n">
+        <v>20319280</v>
+      </c>
+      <c r="Y15" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>499000</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>20319280</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>135</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>59.6</t>
+          <t>43.47</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G16" s="1" t="n">
@@ -1430,31 +1646,49 @@
       <c r="U16" t="n">
         <v>22528800</v>
       </c>
+      <c r="V16" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W16" s="2" t="n">
+        <v>469000</v>
+      </c>
+      <c r="X16" t="n">
+        <v>20387430</v>
+      </c>
+      <c r="Y16" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>469000</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>20387430</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>204</t>
+          <t>28</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>68.24</t>
+          <t>40.02</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G17" s="1" t="n">
@@ -1502,31 +1736,49 @@
       <c r="U17" t="n">
         <v>24293440</v>
       </c>
+      <c r="V17" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W17" s="2" t="n">
+        <v>514000</v>
+      </c>
+      <c r="X17" t="n">
+        <v>20570280</v>
+      </c>
+      <c r="Y17" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>514000</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>20570280</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>203</t>
+          <t>45</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>59.6</t>
+          <t>41.26</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G18" s="1" t="n">
@@ -1574,31 +1826,49 @@
       <c r="U18" t="n">
         <v>22350000</v>
       </c>
+      <c r="V18" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W18" s="2" t="n">
+        <v>499000</v>
+      </c>
+      <c r="X18" t="n">
+        <v>20588740</v>
+      </c>
+      <c r="Y18" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>499000</v>
+      </c>
+      <c r="AA18" t="n">
+        <v>20588740</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>39</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>68.24</t>
+          <t>41.26</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G19" s="1" t="n">
@@ -1646,31 +1916,49 @@
       <c r="U19" t="n">
         <v>24156960</v>
       </c>
+      <c r="V19" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W19" s="2" t="n">
+        <v>504000</v>
+      </c>
+      <c r="X19" t="n">
+        <v>20795040</v>
+      </c>
+      <c r="Y19" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>504000</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>20795040</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>197</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>59.6</t>
+          <t>40.6</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G20" s="1" t="n">
@@ -1718,31 +2006,49 @@
       <c r="U20" t="n">
         <v>20442800</v>
       </c>
+      <c r="V20" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W20" s="2" t="n">
+        <v>514000</v>
+      </c>
+      <c r="X20" t="n">
+        <v>20868400</v>
+      </c>
+      <c r="Y20" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>514000</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>20868400</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>193</t>
+          <t>37</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>59.6</t>
+          <t>40.49</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t xml:space="preserve">8  </t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t xml:space="preserve">1 </t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">4 </t>
         </is>
       </c>
       <c r="G21" s="1" t="n">
@@ -1790,31 +2096,49 @@
       <c r="U21" t="n">
         <v>20740800</v>
       </c>
+      <c r="V21" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W21" s="2" t="n">
+        <v>516000</v>
+      </c>
+      <c r="X21" t="n">
+        <v>20892840</v>
+      </c>
+      <c r="Y21" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>516000</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>20892840</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>190</t>
+          <t>31</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>64.47</t>
+          <t>40.49</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G22" s="1" t="n">
@@ -1862,31 +2186,49 @@
       <c r="U22" t="n">
         <v>22500030</v>
       </c>
+      <c r="V22" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W22" s="2" t="n">
+        <v>516000</v>
+      </c>
+      <c r="X22" t="n">
+        <v>20892840</v>
+      </c>
+      <c r="Y22" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>516000</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>20892840</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>34</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>91.74</t>
+          <t>40.72</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G23" s="1" t="n">
@@ -1934,11 +2276,29 @@
       <c r="U23" t="n">
         <v>32659440</v>
       </c>
+      <c r="V23" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W23" s="2" t="n">
+        <v>514000</v>
+      </c>
+      <c r="X23" t="n">
+        <v>20930080</v>
+      </c>
+      <c r="Y23" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>514000</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>20930080</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>186</t>
+          <t>129</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1948,12 +2308,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>43.96</t>
+          <t>43.47</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2006,11 +2366,29 @@
       <c r="U24" t="n">
         <v>15825600</v>
       </c>
+      <c r="V24" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W24" s="2" t="n">
+        <v>484000</v>
+      </c>
+      <c r="X24" t="n">
+        <v>21039480</v>
+      </c>
+      <c r="Y24" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>484000</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>21039480</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>185</t>
+          <t>33</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2020,17 +2398,17 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>44.28</t>
+          <t>41.26</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G25" s="1" t="n">
@@ -2078,26 +2456,44 @@
       <c r="U25" t="n">
         <v>16029360</v>
       </c>
+      <c r="V25" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W25" s="2" t="n">
+        <v>514000</v>
+      </c>
+      <c r="X25" t="n">
+        <v>21207640</v>
+      </c>
+      <c r="Y25" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>514000</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>21207640</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>184</t>
+          <t>117</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>64.47</t>
+          <t>42.46</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2150,11 +2546,29 @@
       <c r="U26" t="n">
         <v>23144730</v>
       </c>
+      <c r="V26" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W26" s="2" t="n">
+        <v>504000</v>
+      </c>
+      <c r="X26" t="n">
+        <v>21399840</v>
+      </c>
+      <c r="Y26" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>504000</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>21399840</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>182</t>
+          <t>99</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2164,12 +2578,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>37.02</t>
+          <t>42.46</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2222,31 +2636,49 @@
       <c r="U27" t="n">
         <v>14770980</v>
       </c>
+      <c r="V27" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W27" s="2" t="n">
+        <v>504000</v>
+      </c>
+      <c r="X27" t="n">
+        <v>21399840</v>
+      </c>
+      <c r="Y27" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>504000</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>21399840</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>181</t>
+          <t>26</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>91.74</t>
+          <t>44.5</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G28" s="1" t="n">
@@ -2294,11 +2726,29 @@
       <c r="U28" t="n">
         <v>33943800</v>
       </c>
+      <c r="V28" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W28" s="2" t="n">
+        <v>484000</v>
+      </c>
+      <c r="X28" t="n">
+        <v>21538000</v>
+      </c>
+      <c r="Y28" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>484000</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>21538000</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>180</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2308,17 +2758,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>43.96</t>
+          <t>44.5</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">5  </t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G29" s="1" t="n">
@@ -2366,11 +2816,29 @@
       <c r="U29" t="n">
         <v>16572920</v>
       </c>
+      <c r="V29" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W29" s="2" t="n">
+        <v>484000</v>
+      </c>
+      <c r="X29" t="n">
+        <v>21538000</v>
+      </c>
+      <c r="Y29" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>484000</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>21538000</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>179</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2380,17 +2848,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>44.28</t>
+          <t>44.5</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">4  </t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G30" s="1" t="n">
@@ -2438,31 +2906,49 @@
       <c r="U30" t="n">
         <v>16737840</v>
       </c>
+      <c r="V30" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W30" s="2" t="n">
+        <v>484000</v>
+      </c>
+      <c r="X30" t="n">
+        <v>21538000</v>
+      </c>
+      <c r="Y30" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>484000</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>21538000</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>178</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>64.47</t>
+          <t>44.5</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G31" s="1" t="n">
@@ -2510,11 +2996,29 @@
       <c r="U31" t="n">
         <v>23338140</v>
       </c>
+      <c r="V31" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W31" s="2" t="n">
+        <v>484000</v>
+      </c>
+      <c r="X31" t="n">
+        <v>21538000</v>
+      </c>
+      <c r="Y31" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>484000</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>21538000</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>176</t>
+          <t>32</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2524,17 +3028,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>37.02</t>
+          <t>46.24</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">1 </t>
         </is>
       </c>
       <c r="G32" s="1" t="n">
@@ -2582,31 +3086,49 @@
       <c r="U32" t="n">
         <v>13993560</v>
       </c>
+      <c r="V32" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W32" s="2" t="n">
+        <v>468500</v>
+      </c>
+      <c r="X32" t="n">
+        <v>21663440</v>
+      </c>
+      <c r="Y32" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>468500</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>21663440</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>175</t>
+          <t>270</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>91.74</t>
+          <t>46.06</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">9  </t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G33" s="1" t="n">
@@ -2654,31 +3176,49 @@
       <c r="U33" t="n">
         <v>34310760</v>
       </c>
+      <c r="V33" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W33" s="2" t="n">
+        <v>479000</v>
+      </c>
+      <c r="X33" t="n">
+        <v>22062740</v>
+      </c>
+      <c r="Y33" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>479000</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>22062740</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>174</t>
+          <t>236</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>43.96</t>
+          <t>52.48</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">2  </t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G34" s="1" t="n">
@@ -2726,31 +3266,49 @@
       <c r="U34" t="n">
         <v>16572920</v>
       </c>
+      <c r="V34" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W34" s="2" t="n">
+        <v>435000</v>
+      </c>
+      <c r="X34" t="n">
+        <v>22828800</v>
+      </c>
+      <c r="Y34" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>435000</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>22828800</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>173</t>
+          <t>53</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>44.28</t>
+          <t>56.36</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">2  </t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="G35" s="1" t="n">
@@ -2798,11 +3356,29 @@
       <c r="U35" t="n">
         <v>16737840</v>
       </c>
+      <c r="V35" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W35" s="2" t="n">
+        <v>437000</v>
+      </c>
+      <c r="X35" t="n">
+        <v>24629320</v>
+      </c>
+      <c r="Y35" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>437000</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>24629320</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>172</t>
+          <t>81</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2812,17 +3388,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>64.47</t>
+          <t>58.44</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="G36" s="1" t="n">
@@ -2870,31 +3446,49 @@
       <c r="U36" t="n">
         <v>23338140</v>
       </c>
+      <c r="V36" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W36" s="2" t="n">
+        <v>471000</v>
+      </c>
+      <c r="X36" t="n">
+        <v>27525240</v>
+      </c>
+      <c r="Y36" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>471000</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>27525240</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>170</t>
+          <t>71</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>37.02</t>
+          <t>56.61</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="G37" s="1" t="n">
@@ -2942,31 +3536,49 @@
       <c r="U37" t="n">
         <v>13623360</v>
       </c>
+      <c r="V37" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W37" s="2" t="n">
+        <v>487000</v>
+      </c>
+      <c r="X37" t="n">
+        <v>27569070</v>
+      </c>
+      <c r="Y37" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>487000</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>27569070</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>169</t>
+          <t>263</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>91.74</t>
+          <t>59.62</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G38" s="1" t="n">
@@ -3014,31 +3626,49 @@
       <c r="U38" t="n">
         <v>34310760</v>
       </c>
+      <c r="V38" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W38" s="2" t="n">
+        <v>470000</v>
+      </c>
+      <c r="X38" t="n">
+        <v>28021400</v>
+      </c>
+      <c r="Y38" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>470000</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>28021400</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>167</t>
+          <t>208</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>44.28</t>
+          <t>65.55</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">9 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G39" s="1" t="n">
@@ -3086,11 +3716,29 @@
       <c r="U39" t="n">
         <v>16737840</v>
       </c>
+      <c r="V39" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W39" s="2" t="n">
+        <v>442000</v>
+      </c>
+      <c r="X39" t="n">
+        <v>28973100</v>
+      </c>
+      <c r="Y39" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>442000</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>28973100</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>166</t>
+          <t>190</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3100,17 +3748,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>65.55</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G40" s="1" t="n">
@@ -3158,31 +3806,49 @@
       <c r="U40" t="n">
         <v>22961660</v>
       </c>
+      <c r="V40" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W40" s="2" t="n">
+        <v>442000</v>
+      </c>
+      <c r="X40" t="n">
+        <v>28973100</v>
+      </c>
+      <c r="Y40" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>442000</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>28973100</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>164</t>
+          <t>137</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>36.27</t>
+          <t>70.18</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 </t>
+          <t xml:space="preserve">2  </t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">4 </t>
         </is>
       </c>
       <c r="G41" s="1" t="n">
@@ -3230,26 +3896,44 @@
       <c r="U41" t="n">
         <v>14435460</v>
       </c>
+      <c r="V41" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W41" s="2" t="n">
+        <v>415000</v>
+      </c>
+      <c r="X41" t="n">
+        <v>29124700</v>
+      </c>
+      <c r="Y41" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>415000</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>29124700</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>163</t>
+          <t>125</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>90.15</t>
+          <t>63.98</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -3302,31 +3986,49 @@
       <c r="U42" t="n">
         <v>33716100</v>
       </c>
+      <c r="V42" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W42" s="2" t="n">
+        <v>456000</v>
+      </c>
+      <c r="X42" t="n">
+        <v>29174880</v>
+      </c>
+      <c r="Y42" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>456000</v>
+      </c>
+      <c r="AA42" t="n">
+        <v>29174880</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>162</t>
+          <t>214</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>43.3</t>
+          <t>66.67</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G43" s="1" t="n">
@@ -3374,26 +4076,44 @@
       <c r="U43" t="n">
         <v>16324100</v>
       </c>
+      <c r="V43" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W43" s="2" t="n">
+        <v>440000</v>
+      </c>
+      <c r="X43" t="n">
+        <v>29334800</v>
+      </c>
+      <c r="Y43" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>440000</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>29334800</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>161</t>
+          <t>119</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>42.72</t>
+          <t>63.98</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t xml:space="preserve">8 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -3446,11 +4166,29 @@
       <c r="U44" t="n">
         <v>16148160</v>
       </c>
+      <c r="V44" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W44" s="2" t="n">
+        <v>459000</v>
+      </c>
+      <c r="X44" t="n">
+        <v>29366820</v>
+      </c>
+      <c r="Y44" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z44" t="n">
+        <v>459000</v>
+      </c>
+      <c r="AA44" t="n">
+        <v>29366820</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>160</t>
+          <t>89</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3460,12 +4198,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>67.91</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t xml:space="preserve">7 </t>
+          <t xml:space="preserve">2  </t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -3518,31 +4256,49 @@
       <c r="U45" t="n">
         <v>22961660</v>
       </c>
+      <c r="V45" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W45" s="2" t="n">
+        <v>434000</v>
+      </c>
+      <c r="X45" t="n">
+        <v>29472940</v>
+      </c>
+      <c r="Y45" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z45" t="n">
+        <v>434000</v>
+      </c>
+      <c r="AA45" t="n">
+        <v>29472940</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>157</t>
+          <t>303</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>90.15</t>
+          <t>67.65</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
+          <t xml:space="preserve">7  </t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
           <t xml:space="preserve">7 </t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G46" s="1" t="n">
@@ -3590,31 +4346,49 @@
       <c r="U46" t="n">
         <v>33716100</v>
       </c>
+      <c r="V46" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W46" s="2" t="n">
+        <v>443000</v>
+      </c>
+      <c r="X46" t="n">
+        <v>29968950</v>
+      </c>
+      <c r="Y46" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z46" t="n">
+        <v>443000</v>
+      </c>
+      <c r="AA46" t="n">
+        <v>29968950</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>155</t>
+          <t>249</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>42.72</t>
+          <t>68.02</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t xml:space="preserve">7 </t>
+          <t xml:space="preserve">5  </t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G47" s="1" t="n">
@@ -3662,11 +4436,29 @@
       <c r="U47" t="n">
         <v>16148160</v>
       </c>
+      <c r="V47" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W47" s="2" t="n">
+        <v>443000</v>
+      </c>
+      <c r="X47" t="n">
+        <v>30132860</v>
+      </c>
+      <c r="Y47" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z47" t="n">
+        <v>443000</v>
+      </c>
+      <c r="AA47" t="n">
+        <v>30132860</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>244</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3676,17 +4468,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>68.02</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
+          <t xml:space="preserve">4  </t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
           <t xml:space="preserve">6 </t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G48" s="1" t="n">
@@ -3734,31 +4526,49 @@
       <c r="U48" t="n">
         <v>23088520</v>
       </c>
+      <c r="V48" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W48" s="2" t="n">
+        <v>443000</v>
+      </c>
+      <c r="X48" t="n">
+        <v>30132860</v>
+      </c>
+      <c r="Y48" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z48" t="n">
+        <v>443000</v>
+      </c>
+      <c r="AA48" t="n">
+        <v>30132860</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>152</t>
+          <t>239</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>36.27</t>
+          <t>68.02</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
+          <t xml:space="preserve">3  </t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
           <t xml:space="preserve">6 </t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t xml:space="preserve">3 </t>
         </is>
       </c>
       <c r="G49" s="1" t="n">
@@ -3806,31 +4616,49 @@
       <c r="U49" t="n">
         <v>14508000</v>
       </c>
+      <c r="V49" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W49" s="2" t="n">
+        <v>443000</v>
+      </c>
+      <c r="X49" t="n">
+        <v>30132860</v>
+      </c>
+      <c r="Y49" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z49" t="n">
+        <v>443000</v>
+      </c>
+      <c r="AA49" t="n">
+        <v>30132860</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>151</t>
+          <t>70</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>90.15</t>
+          <t>69.82</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t xml:space="preserve">6 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="G50" s="1" t="n">
@@ -3878,31 +4706,49 @@
       <c r="U50" t="n">
         <v>33896400</v>
       </c>
+      <c r="V50" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W50" s="2" t="n">
+        <v>435000</v>
+      </c>
+      <c r="X50" t="n">
+        <v>30371700</v>
+      </c>
+      <c r="Y50" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>435000</v>
+      </c>
+      <c r="AA50" t="n">
+        <v>30371700</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>149</t>
+          <t>65</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>42.72</t>
+          <t>69.82</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t xml:space="preserve">6 </t>
+          <t xml:space="preserve">5  </t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="G51" s="1" t="n">
@@ -3950,11 +4796,29 @@
       <c r="U51" t="n">
         <v>16233600</v>
       </c>
+      <c r="V51" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W51" s="2" t="n">
+        <v>435000</v>
+      </c>
+      <c r="X51" t="n">
+        <v>30371700</v>
+      </c>
+      <c r="Y51" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z51" t="n">
+        <v>435000</v>
+      </c>
+      <c r="AA51" t="n">
+        <v>30371700</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>60</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -3964,17 +4828,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>69.82</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t xml:space="preserve">5 </t>
+          <t xml:space="preserve">4  </t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="G52" s="1" t="n">
@@ -4022,11 +4886,29 @@
       <c r="U52" t="n">
         <v>23088520</v>
       </c>
+      <c r="V52" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W52" s="2" t="n">
+        <v>435000</v>
+      </c>
+      <c r="X52" t="n">
+        <v>30371700</v>
+      </c>
+      <c r="Y52" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z52" t="n">
+        <v>435000</v>
+      </c>
+      <c r="AA52" t="n">
+        <v>30371700</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>235</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4036,17 +4918,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>72.56</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">2  </t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G53" s="1" t="n">
@@ -4094,31 +4976,49 @@
       <c r="U53" t="n">
         <v>23088520</v>
       </c>
+      <c r="V53" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W53" s="2" t="n">
+        <v>421000</v>
+      </c>
+      <c r="X53" t="n">
+        <v>30547760</v>
+      </c>
+      <c r="Y53" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z53" t="n">
+        <v>421000</v>
+      </c>
+      <c r="AA53" t="n">
+        <v>30547760</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>140</t>
+          <t>75</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>36.27</t>
+          <t>70.82</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t xml:space="preserve">4 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">2 </t>
         </is>
       </c>
       <c r="G54" s="1" t="n">
@@ -4166,11 +5066,29 @@
       <c r="U54" t="n">
         <v>14508000</v>
       </c>
+      <c r="V54" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W54" s="2" t="n">
+        <v>433000</v>
+      </c>
+      <c r="X54" t="n">
+        <v>30665060</v>
+      </c>
+      <c r="Y54" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z54" t="n">
+        <v>433000</v>
+      </c>
+      <c r="AA54" t="n">
+        <v>30665060</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>136</t>
+          <t>161</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4180,17 +5098,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>70.18</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">4 </t>
         </is>
       </c>
       <c r="G55" s="1" t="n">
@@ -4238,31 +5156,49 @@
       <c r="U55" t="n">
         <v>23088520</v>
       </c>
+      <c r="V55" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W55" s="2" t="n">
+        <v>439000</v>
+      </c>
+      <c r="X55" t="n">
+        <v>30809020</v>
+      </c>
+      <c r="Y55" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z55" t="n">
+        <v>439000</v>
+      </c>
+      <c r="AA55" t="n">
+        <v>30809020</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>173</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>36.27</t>
+          <t>71.28</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">4 </t>
         </is>
       </c>
       <c r="G56" s="1" t="n">
@@ -4310,11 +5246,29 @@
       <c r="U56" t="n">
         <v>14508000</v>
       </c>
+      <c r="V56" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W56" s="2" t="n">
+        <v>433000</v>
+      </c>
+      <c r="X56" t="n">
+        <v>30864240</v>
+      </c>
+      <c r="Y56" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z56" t="n">
+        <v>433000</v>
+      </c>
+      <c r="AA56" t="n">
+        <v>30864240</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>259</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4324,17 +5278,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>70.05</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G57" s="1" t="n">
@@ -4382,31 +5336,49 @@
       <c r="U57" t="n">
         <v>22961660</v>
       </c>
+      <c r="V57" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W57" s="2" t="n">
+        <v>441000</v>
+      </c>
+      <c r="X57" t="n">
+        <v>30892050</v>
+      </c>
+      <c r="Y57" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z57" t="n">
+        <v>441000</v>
+      </c>
+      <c r="AA57" t="n">
+        <v>30892050</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>128</t>
+          <t>167</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>36.27</t>
+          <t>71.28</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">4 </t>
         </is>
       </c>
       <c r="G58" s="1" t="n">
@@ -4454,11 +5426,29 @@
       <c r="U58" t="n">
         <v>14435460</v>
       </c>
+      <c r="V58" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W58" s="2" t="n">
+        <v>437000</v>
+      </c>
+      <c r="X58" t="n">
+        <v>31149360</v>
+      </c>
+      <c r="Y58" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z58" t="n">
+        <v>437000</v>
+      </c>
+      <c r="AA58" t="n">
+        <v>31149360</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>127</t>
+          <t>195</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4468,17 +5458,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>90.15</t>
+          <t>81.67</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G59" s="1" t="n">
@@ -4526,31 +5516,49 @@
       <c r="U59" t="n">
         <v>33716100</v>
       </c>
+      <c r="V59" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W59" s="2" t="n">
+        <v>440000</v>
+      </c>
+      <c r="X59" t="n">
+        <v>35934800</v>
+      </c>
+      <c r="Y59" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z59" t="n">
+        <v>440000</v>
+      </c>
+      <c r="AA59" t="n">
+        <v>35934800</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>125</t>
+          <t>219</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>42.72</t>
+          <t>83.17</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">5 </t>
         </is>
       </c>
       <c r="G60" s="1" t="n">
@@ -4598,31 +5606,49 @@
       <c r="U60" t="n">
         <v>16062720</v>
       </c>
+      <c r="V60" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W60" s="2" t="n">
+        <v>438000</v>
+      </c>
+      <c r="X60" t="n">
+        <v>36428460</v>
+      </c>
+      <c r="Y60" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z60" t="n">
+        <v>438000</v>
+      </c>
+      <c r="AA60" t="n">
+        <v>36428460</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>121</t>
+          <t>282</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>63.43</t>
+          <t>96.35</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t xml:space="preserve">1 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t xml:space="preserve">3 </t>
+          <t xml:space="preserve">7 </t>
         </is>
       </c>
       <c r="G61" s="1" t="n">
@@ -4670,31 +5696,49 @@
       <c r="U61" t="n">
         <v>21693060</v>
       </c>
+      <c r="V61" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W61" s="2" t="n">
+        <v>407000</v>
+      </c>
+      <c r="X61" t="n">
+        <v>39214450</v>
+      </c>
+      <c r="Y61" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z61" t="n">
+        <v>407000</v>
+      </c>
+      <c r="AA61" t="n">
+        <v>39214450</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>118</t>
+          <t>237</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>67.1</t>
+          <t>94.31</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G62" s="1" t="n">
@@ -4742,31 +5786,49 @@
       <c r="U62" t="n">
         <v>23686300</v>
       </c>
+      <c r="V62" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W62" s="2" t="n">
+        <v>422000</v>
+      </c>
+      <c r="X62" t="n">
+        <v>39798820</v>
+      </c>
+      <c r="Y62" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z62" t="n">
+        <v>422000</v>
+      </c>
+      <c r="AA62" t="n">
+        <v>39798820</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>117</t>
+          <t>262</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>38.56</t>
+          <t>95.83</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G63" s="1" t="n">
@@ -4814,31 +5876,49 @@
       <c r="U63" t="n">
         <v>14691360</v>
       </c>
+      <c r="V63" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W63" s="2" t="n">
+        <v>416000</v>
+      </c>
+      <c r="X63" t="n">
+        <v>39865280</v>
+      </c>
+      <c r="Y63" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z63" t="n">
+        <v>416000</v>
+      </c>
+      <c r="AA63" t="n">
+        <v>39865280</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>116</t>
+          <t>312</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>38.41</t>
+          <t>99.83</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t xml:space="preserve">12 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">7 </t>
         </is>
       </c>
       <c r="G64" s="1" t="n">
@@ -4886,31 +5966,49 @@
       <c r="U64" t="n">
         <v>14634210</v>
       </c>
+      <c r="V64" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W64" s="2" t="n">
+        <v>405000</v>
+      </c>
+      <c r="X64" t="n">
+        <v>40431150</v>
+      </c>
+      <c r="Y64" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z64" t="n">
+        <v>405000</v>
+      </c>
+      <c r="AA64" t="n">
+        <v>40431150</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>256</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>39.55</t>
+          <t>96.27</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">6  </t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G65" s="1" t="n">
@@ -4958,31 +6056,49 @@
       <c r="U65" t="n">
         <v>15464050</v>
       </c>
+      <c r="V65" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W65" s="2" t="n">
+        <v>422000</v>
+      </c>
+      <c r="X65" t="n">
+        <v>40625940</v>
+      </c>
+      <c r="Y65" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z65" t="n">
+        <v>422000</v>
+      </c>
+      <c r="AA65" t="n">
+        <v>40625940</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>113</t>
+          <t>241</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>67.1</t>
+          <t>96.27</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G66" s="1" t="n">
@@ -5030,31 +6146,49 @@
       <c r="U66" t="n">
         <v>24357300</v>
       </c>
+      <c r="V66" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W66" s="2" t="n">
+        <v>422000</v>
+      </c>
+      <c r="X66" t="n">
+        <v>40625940</v>
+      </c>
+      <c r="Y66" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z66" t="n">
+        <v>422000</v>
+      </c>
+      <c r="AA66" t="n">
+        <v>40625940</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>112</t>
+          <t>266</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>38.56</t>
+          <t>97.83</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G67" s="1" t="n">
@@ -5102,26 +6236,44 @@
       <c r="U67" t="n">
         <v>15346880</v>
       </c>
+      <c r="V67" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W67" s="2" t="n">
+        <v>416000</v>
+      </c>
+      <c r="X67" t="n">
+        <v>40697280</v>
+      </c>
+      <c r="Y67" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z67" t="n">
+        <v>416000</v>
+      </c>
+      <c r="AA67" t="n">
+        <v>40697280</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>64</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>38.41</t>
+          <t>99.45</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">5  </t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -5174,11 +6326,29 @@
       <c r="U68" t="n">
         <v>15210360</v>
       </c>
+      <c r="V68" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W68" s="2" t="n">
+        <v>419000</v>
+      </c>
+      <c r="X68" t="n">
+        <v>41669550</v>
+      </c>
+      <c r="Y68" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z68" t="n">
+        <v>419000</v>
+      </c>
+      <c r="AA68" t="n">
+        <v>41669550</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>59</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5188,12 +6358,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>93.18</t>
+          <t>99.45</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t xml:space="preserve">11 </t>
+          <t xml:space="preserve">4  </t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -5246,26 +6416,44 @@
       <c r="U69" t="n">
         <v>34010700</v>
       </c>
+      <c r="V69" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W69" s="2" t="n">
+        <v>419000</v>
+      </c>
+      <c r="X69" t="n">
+        <v>41669550</v>
+      </c>
+      <c r="Y69" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z69" t="n">
+        <v>419000</v>
+      </c>
+      <c r="AA69" t="n">
+        <v>41669550</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>54</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>39.55</t>
+          <t>99.45</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">3  </t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -5318,26 +6506,44 @@
       <c r="U70" t="n">
         <v>15464050</v>
       </c>
+      <c r="V70" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W70" s="2" t="n">
+        <v>419000</v>
+      </c>
+      <c r="X70" t="n">
+        <v>41669550</v>
+      </c>
+      <c r="Y70" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z70" t="n">
+        <v>419000</v>
+      </c>
+      <c r="AA70" t="n">
+        <v>41669550</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>79</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>67.1</t>
+          <t>100.92</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">8  </t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -5390,31 +6596,49 @@
       <c r="U71" t="n">
         <v>24558600</v>
       </c>
+      <c r="V71" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W71" s="2" t="n">
+        <v>413000</v>
+      </c>
+      <c r="X71" t="n">
+        <v>41679960</v>
+      </c>
+      <c r="Y71" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z71" t="n">
+        <v>413000</v>
+      </c>
+      <c r="AA71" t="n">
+        <v>41679960</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>257</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>38.56</t>
+          <t>95.83</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t xml:space="preserve">10 </t>
+          <t xml:space="preserve">7  </t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t xml:space="preserve">2 </t>
+          <t xml:space="preserve">6 </t>
         </is>
       </c>
       <c r="G72" s="1" t="n">
@@ -5461,6 +6685,24 @@
       </c>
       <c r="U72" t="n">
         <v>15346880</v>
+      </c>
+      <c r="V72" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="W72" s="2" t="n">
+        <v>443000</v>
+      </c>
+      <c r="X72" t="n">
+        <v>42452690</v>
+      </c>
+      <c r="Y72" s="1" t="n">
+        <v>45634</v>
+      </c>
+      <c r="Z72" t="n">
+        <v>443000</v>
+      </c>
+      <c r="AA72" t="n">
+        <v>42452690</v>
       </c>
     </row>
     <row r="73">

</xml_diff>